<commit_message>
Initial commit of companies in Chennai
</commit_message>
<xml_diff>
--- a/CompaniesInChennai_V1.0.xlsx
+++ b/CompaniesInChennai_V1.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ChennaiCompaniesList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B482D42-E51E-45CB-87B1-DB5A53DECB0B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D05614B-64BF-498B-B216-A2487AB86E4D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2719,7 +2719,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:J2"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -9021,22 +9021,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A178:J178"/>
-    <mergeCell ref="A181:J181"/>
-    <mergeCell ref="A188:J188"/>
-    <mergeCell ref="A195:J195"/>
-    <mergeCell ref="A239:J239"/>
-    <mergeCell ref="A209:J209"/>
-    <mergeCell ref="A103:J103"/>
-    <mergeCell ref="A137:J137"/>
-    <mergeCell ref="A141:J141"/>
-    <mergeCell ref="A147:J147"/>
-    <mergeCell ref="A152:J152"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A35:J35"/>
-    <mergeCell ref="A65:J65"/>
-    <mergeCell ref="A77:J77"/>
-    <mergeCell ref="A96:J96"/>
     <mergeCell ref="A161:J161"/>
     <mergeCell ref="A165:J165"/>
     <mergeCell ref="A169:J169"/>
@@ -9046,6 +9030,22 @@
     <mergeCell ref="A133:J133"/>
     <mergeCell ref="A159:J159"/>
     <mergeCell ref="A156:J156"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A35:J35"/>
+    <mergeCell ref="A65:J65"/>
+    <mergeCell ref="A77:J77"/>
+    <mergeCell ref="A96:J96"/>
+    <mergeCell ref="A103:J103"/>
+    <mergeCell ref="A137:J137"/>
+    <mergeCell ref="A141:J141"/>
+    <mergeCell ref="A147:J147"/>
+    <mergeCell ref="A152:J152"/>
+    <mergeCell ref="A178:J178"/>
+    <mergeCell ref="A181:J181"/>
+    <mergeCell ref="A188:J188"/>
+    <mergeCell ref="A195:J195"/>
+    <mergeCell ref="A239:J239"/>
+    <mergeCell ref="A209:J209"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>